<commit_message>
Added region and interval definitions
</commit_message>
<xml_diff>
--- a/files/integration_template.xlsx
+++ b/files/integration_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="sectormodel_inputs" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,9 @@
     <sheet name="parameters" sheetId="3" r:id="rId3"/>
     <sheet name="intervals" sheetId="5" r:id="rId4"/>
     <sheet name="scenario" sheetId="6" r:id="rId5"/>
-    <sheet name="interventions" sheetId="4" r:id="rId6"/>
+    <sheet name="region_definitions" sheetId="7" r:id="rId6"/>
+    <sheet name="scenario_definitions" sheetId="8" r:id="rId7"/>
+    <sheet name="interventions" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
   <si>
     <t>name</t>
   </si>
@@ -110,6 +112,9 @@
   </si>
   <si>
     <t>value</t>
+  </si>
+  <si>
+    <t>filename</t>
   </si>
 </sst>
 </file>
@@ -573,7 +578,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -600,10 +605,62 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added initial condition system tabs to xlsx
</commit_message>
<xml_diff>
--- a/files/integration_template.xlsx
+++ b/files/integration_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="sectormodel_inputs" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="region_definitions" sheetId="7" r:id="rId6"/>
     <sheet name="scenario_definitions" sheetId="8" r:id="rId7"/>
     <sheet name="interventions" sheetId="4" r:id="rId8"/>
+    <sheet name="initial_system" sheetId="9" r:id="rId9"/>
+    <sheet name="initial_conditions" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -115,6 +117,18 @@
   </si>
   <si>
     <t>filename</t>
+  </si>
+  <si>
+    <t>intervention_name</t>
+  </si>
+  <si>
+    <t>build_year</t>
+  </si>
+  <si>
+    <t>parameter_name</t>
+  </si>
+  <si>
+    <t>initial_value</t>
   </si>
 </sst>
 </file>
@@ -462,6 +476,32 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
@@ -659,7 +699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
@@ -737,4 +777,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Typos, reordered xlsx tabs
</commit_message>
<xml_diff>
--- a/files/integration_template.xlsx
+++ b/files/integration_template.xlsx
@@ -9,19 +9,20 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="9"/>
+    <workbookView xWindow="38400" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
-    <sheet name="sectormodel_inputs" sheetId="1" r:id="rId1"/>
-    <sheet name="sectormodel_outputs" sheetId="2" r:id="rId2"/>
-    <sheet name="parameters" sheetId="3" r:id="rId3"/>
-    <sheet name="intervals" sheetId="5" r:id="rId4"/>
-    <sheet name="scenario" sheetId="6" r:id="rId5"/>
-    <sheet name="region_definitions" sheetId="7" r:id="rId6"/>
-    <sheet name="scenario_definitions" sheetId="8" r:id="rId7"/>
-    <sheet name="interventions" sheetId="4" r:id="rId8"/>
-    <sheet name="initial_system" sheetId="9" r:id="rId9"/>
-    <sheet name="initial_conditions" sheetId="10" r:id="rId10"/>
+    <sheet name="region_definitions" sheetId="7" r:id="rId1"/>
+    <sheet name="interval_definitions" sheetId="11" r:id="rId2"/>
+    <sheet name="intervals" sheetId="5" r:id="rId3"/>
+    <sheet name="sectormodel_inputs" sheetId="1" r:id="rId4"/>
+    <sheet name="sectormodel_outputs" sheetId="2" r:id="rId5"/>
+    <sheet name="parameters" sheetId="3" r:id="rId6"/>
+    <sheet name="interventions" sheetId="4" r:id="rId7"/>
+    <sheet name="initial_system" sheetId="9" r:id="rId8"/>
+    <sheet name="initial_conditions" sheetId="10" r:id="rId9"/>
+    <sheet name="scenario" sheetId="6" r:id="rId10"/>
+    <sheet name="scenario_definitions" sheetId="8" r:id="rId11"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
   <si>
     <t>name</t>
   </si>
@@ -443,9 +444,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -476,33 +610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D1"/>
   <sheetViews>
@@ -537,7 +645,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1"/>
   <sheetViews>
@@ -588,114 +696,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S1"/>
   <sheetViews>
@@ -779,7 +780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -803,4 +804,30 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>